<commit_message>
und noch mehr plots
</commit_message>
<xml_diff>
--- a/01_studies/01_Laborstudie ProVisioNET/R script/sri coding/data/Coding_SRI.xlsx
+++ b/01_studies/01_Laborstudie ProVisioNET/R script/sri coding/data/Coding_SRI.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mk99feta\OneDrive\Dokumente\GitHub\Mandy-PhD\01_studies\01_Laborstudie ProVisioNET\R script\sri coding\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/505858402c07da9d/Dokumente/GitHub/Mandy-PhD/01_studies/01_Laborstudie ProVisioNET/R script/sri coding/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="14_{BCBBD0FC-4723-442C-8B9A-91266470354A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{D358537F-D4A0-4E5D-BE26-6DF74DBBE246}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{534A4DE0-5ADC-4586-BD79-1300FA56E80D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" xr2:uid="{E076B5D5-D199-4D8E-A2C0-E3EC9D7FADC9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="1" xr2:uid="{E076B5D5-D199-4D8E-A2C0-E3EC9D7FADC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Rating Novices" sheetId="3" r:id="rId1"/>
@@ -508,7 +508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{403ECED8-55F4-4FC6-AC8C-3350BC92FAB2}">
   <dimension ref="A1:H228"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A65" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -4988,8 +4988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D8D7183-98EA-4827-B19F-C9663A3867CB}">
   <dimension ref="A1:H147"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5153,7 +5153,7 @@
         <v>8</v>
       </c>
       <c r="D8" s="1">
-        <v>0</v>
+        <v>-99</v>
       </c>
       <c r="E8" s="1">
         <v>-99</v>

</xml_diff>